<commit_message>
-update permission -fix incident running no -fix password after create user -sla tempalte nullable for service level
</commit_message>
<xml_diff>
--- a/database/seeders/excel/permission.xlsx
+++ b/database/seeders/excel/permission.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\niise_helpdesk\be\database\seeders\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmadnajmibinsidek/Developer/niise-helpdesk/backend/database/seeders/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C95411B-9EB5-A443-8967-CDAEC075E0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="23040" windowHeight="12120"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="48">
   <si>
     <t>dashboard</t>
   </si>
@@ -159,13 +161,16 @@
   </si>
   <si>
     <t>resolution</t>
+  </si>
+  <si>
+    <t>BTMR,FRONTLINER,JIM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,7 +188,13 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -196,6 +207,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -204,10 +223,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -487,29 +506,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="2" max="2" width="31.375" customWidth="1"/>
-    <col min="3" max="3" width="20.75" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
     <col min="6" max="6" width="21.5" customWidth="1"/>
-    <col min="7" max="9" width="33.25" customWidth="1"/>
+    <col min="7" max="9" width="33.1640625" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -531,7 +553,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -542,7 +564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -565,7 +587,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -588,7 +610,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -602,7 +624,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -625,7 +647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -636,7 +658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -659,7 +681,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -682,7 +704,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -705,7 +727,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -728,7 +750,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -739,7 +761,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -765,7 +787,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -788,7 +810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -799,7 +821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -822,7 +844,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -845,7 +867,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -862,7 +884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -885,7 +907,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -899,7 +921,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -913,7 +935,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -921,13 +943,13 @@
         <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
         <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="F23" t="s">
         <v>3</v>
@@ -936,7 +958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -960,6 +982,7 @@
       </c>
     </row>
   </sheetData>
-  <pageSetup r:id="rId1" orientation="portrait"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update seeder user and role
</commit_message>
<xml_diff>
--- a/database/seeders/excel/permission.xlsx
+++ b/database/seeders/excel/permission.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmadnajmibinsidek/Developer/niise-helpdesk/backend/database/seeders/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C95411B-9EB5-A443-8967-CDAEC075E0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CAA80E-AA83-C34D-94B3-70A9D41C4B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <t>dashboard</t>
   </si>
   <si>
-    <t>JIM,FRONTLINER,BTMR,CONTRACTOR</t>
-  </si>
-  <si>
     <t>system_administration</t>
   </si>
   <si>
@@ -43,9 +40,6 @@
     <t>individual</t>
   </si>
   <si>
-    <t>BTMR</t>
-  </si>
-  <si>
     <t>groups</t>
   </si>
   <si>
@@ -130,30 +124,18 @@
     <t>incident</t>
   </si>
   <si>
-    <t>JIM,FRONTLINER,BTMR</t>
-  </si>
-  <si>
     <t>audit_trails</t>
   </si>
   <si>
     <t>audit-trail</t>
   </si>
   <si>
-    <t>FRONTLINER,BTMR,CONTRACTOR</t>
-  </si>
-  <si>
     <t>reports</t>
   </si>
   <si>
     <t>report</t>
   </si>
   <si>
-    <t>BTMR,CONTRACTOR,FRONTLINER</t>
-  </si>
-  <si>
-    <t>BTMR,CONTRACTOR</t>
-  </si>
-  <si>
     <t>knowledge_base</t>
   </si>
   <si>
@@ -163,7 +145,25 @@
     <t>resolution</t>
   </si>
   <si>
-    <t>BTMR,FRONTLINER,JIM</t>
+    <t>JIM,FRONTLINER,BTMR,CONTRACTOR,SUPER_ADMIN</t>
+  </si>
+  <si>
+    <t>BTMR,FRONTLINER,SUPER_ADMIN</t>
+  </si>
+  <si>
+    <t>BTMR,SUPER_ADMIN</t>
+  </si>
+  <si>
+    <t>FRONTLINER,BTMR,CONTRACTOR,SUPER_ADMIN</t>
+  </si>
+  <si>
+    <t>BTMR,CONTRACTOR,FRONTLINER,SUPER_ADMIN</t>
+  </si>
+  <si>
+    <t>BTMR,FRONTLINER,JIM,SUPER_ADMIN</t>
+  </si>
+  <si>
+    <t>JIM,FRONTLINER,BTMR,SUPER_ADMIN</t>
   </si>
 </sst>
 </file>
@@ -515,18 +515,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="38.1640625" customWidth="1"/>
+    <col min="4" max="4" width="46.83203125" customWidth="1"/>
+    <col min="5" max="5" width="40.33203125" customWidth="1"/>
+    <col min="6" max="6" width="35.1640625" customWidth="1"/>
     <col min="7" max="9" width="33.1640625" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
@@ -539,446 +539,446 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="G7" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="F9" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="G9" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="G10" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="F11" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="G11" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="G12" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E14" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="F14" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="G14" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="H14" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="F15" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="G15" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="F17" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="G17" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="F18" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="G18" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="F19" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="E20" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="F20" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="G20" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E21" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="I22" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="E23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F23" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="G23" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E24" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="F24" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G24" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>